<commit_message>
Verify Home page title
</commit_message>
<xml_diff>
--- a/testdata/gurubankdata.xlsx
+++ b/testdata/gurubankdata.xlsx
@@ -19,12 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>data</t>
   </si>
   <si>
     <t>Manger Id : mngr482972</t>
+  </si>
+  <si>
+    <t>Guru99 Bank Manager HomePage</t>
   </si>
 </sst>
 </file>
@@ -60,10 +63,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -345,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -366,6 +372,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
validating multiple combination of uid and password for login page
</commit_message>
<xml_diff>
--- a/testdata/gurubankdata.xlsx
+++ b/testdata/gurubankdata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>data</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>Guru99 Bank Manager HomePage</t>
+  </si>
+  <si>
+    <t>User or Password is not valid</t>
   </si>
 </sst>
 </file>
@@ -351,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,6 +380,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>